<commit_message>
Rewrite Excel importer. Add parameters, fixes #40.
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/sample_activities_with_variables.xlsx
+++ b/tests/fixtures/excel/sample_activities_with_variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="0" windowWidth="34920" windowHeight="24900" tabRatio="795"/>
+    <workbookView xWindow="7600" yWindow="0" windowWidth="34920" windowHeight="24900" tabRatio="795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global parameters" sheetId="13" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="98">
   <si>
     <t>Database</t>
   </si>
@@ -313,10 +313,10 @@
     <t>Project parameters</t>
   </si>
   <si>
-    <t>Parameters</t>
-  </si>
-  <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>Database parameters</t>
   </si>
 </sst>
 </file>
@@ -835,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -853,7 +853,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>31</v>
@@ -1000,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1018,182 +1018,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:11">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2"/>
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="5">
+        <f>EXP(G3)</f>
+        <v>0.33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5">
+        <f>LN(0.33)</f>
+        <v>-1.1086626245216111</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="C4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="5">
+        <f>G4</f>
+        <v>6.1749999999999999E-2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <f>325*190/1000000</f>
+        <v>6.1749999999999999E-2</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="A5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5">
+        <f>LN(B6)</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5">
-        <f>EXP(G7)</f>
-        <v>0.33</v>
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
       <c r="F7" s="5">
-        <v>2</v>
-      </c>
-      <c r="G7" s="5">
-        <f>LN(0.33)</f>
-        <v>-1.1086626245216111</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="5">
-        <f>G8</f>
-        <v>6.1749999999999999E-2</v>
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+        <v>10</v>
+      </c>
       <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <f>325*190/1000000</f>
-        <v>6.1749999999999999E-2</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="5">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+        <v>10</v>
+      </c>
       <c r="F9" s="5">
-        <v>7</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="4">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+        <v>10</v>
+      </c>
       <c r="F10" s="5">
-        <v>2</v>
-      </c>
-      <c r="G10" s="5">
-        <f>LN(B10)</f>
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F11" s="5">
         <v>4</v>
@@ -1207,7 +1263,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B12">
         <v>0.2</v>
@@ -1226,14 +1282,14 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="5" t="s">
-        <v>63</v>
+      <c r="A13" t="s">
+        <v>73</v>
       </c>
       <c r="B13">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F13" s="5">
         <v>4</v>
@@ -1247,416 +1303,474 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B14">
-        <v>0.2</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f>LN(B14)</f>
+        <v>-1.9732813458514451</v>
+      </c>
+      <c r="H14">
+        <f>LN(3.1581^0.5)</f>
+        <v>0.57498529047162583</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="5">
-        <v>4</v>
-      </c>
-      <c r="J15">
+      <c r="F15">
         <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B16">
-        <v>0.2</v>
+        <v>0.105</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="5">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <f>LN(B16)</f>
+        <v>-2.2537949288246137</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H18" si="0">LN(3.1581^0.5)</f>
+        <v>0.57498529047162583</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" t="s">
-        <v>73</v>
+      <c r="A17" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="B17">
-        <v>0.5</v>
+        <v>4.3799999999999999E-2</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="5">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <f>LN(B17)</f>
+        <v>-3.1281214615997368</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.57498529047162583</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B18">
-        <v>0.13900000000000001</v>
+        <v>3.4799999999999998E-2</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18">
         <v>2</v>
       </c>
       <c r="G18">
         <f>LN(B18)</f>
-        <v>-1.9732813458514451</v>
+        <v>-3.3581378922017087</v>
       </c>
       <c r="H18">
-        <f>LN(3.1581^0.5)</f>
+        <f t="shared" si="0"/>
         <v>0.57498529047162583</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="F19">
-        <v>0</v>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20">
-        <v>0.105</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <f>LN(B20)</f>
-        <v>-2.2537949288246137</v>
-      </c>
-      <c r="H20">
-        <f t="shared" ref="H20:H22" si="0">LN(3.1581^0.5)</f>
-        <v>0.57498529047162583</v>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21">
-        <v>4.3799999999999999E-2</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <f>LN(B21)</f>
-        <v>-3.1281214615997368</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>0.57498529047162583</v>
+      <c r="E21" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22">
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="C22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <f>LN(B22)</f>
-        <v>-3.3581378922017087</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>0.57498529047162583</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>41</v>
+      <c r="E22" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15">
+      <c r="A23" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
-        <v>55</v>
-      </c>
       <c r="E23" t="s">
-        <v>91</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
+      <c r="E24" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="5" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15">
       <c r="A26" s="5" t="s">
-        <v>68</v>
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15">
-      <c r="A27" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="28" spans="1:11" ht="15">
+      <c r="A28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15">
-      <c r="A30" s="5" t="s">
-        <v>85</v>
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="32" spans="1:11" ht="15">
-      <c r="A32" s="1" t="s">
-        <v>2</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="F32" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15">
+      <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" t="s">
+      <c r="F38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>6.1749999999999999E-2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <f>LN(B39)</f>
+        <v>-2.7846613034740506</v>
+      </c>
+      <c r="I39">
+        <v>0.2</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40">
+        <v>6.1749999999999999E-2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <f>LN(B40)</f>
+        <v>-2.7846613034740506</v>
+      </c>
+      <c r="I40">
+        <v>0.2</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41">
+        <v>0.38390999999999997</v>
+      </c>
+      <c r="C41" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" ht="15">
-      <c r="A41" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="15">
-      <c r="A42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>31</v>
+      <c r="D41" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <f>LN(B41)</f>
+        <v>-0.95734712886452289</v>
+      </c>
+      <c r="I41">
+        <v>0.2</v>
+      </c>
+      <c r="M41" t="s">
+        <v>42</v>
+      </c>
+      <c r="N41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>0.38390999999999997</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <f>LN(B42)</f>
+        <v>-0.95734712886452289</v>
+      </c>
+      <c r="I42">
+        <v>0.2</v>
+      </c>
+      <c r="M42" t="s">
+        <v>44</v>
+      </c>
+      <c r="N42" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43">
-        <v>6.1749999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>36</v>
@@ -1665,166 +1779,28 @@
         <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43">
-        <f>LN(B43)</f>
-        <v>-2.7846613034740506</v>
-      </c>
-      <c r="I43">
-        <v>0.2</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44">
-        <v>6.1749999999999999E-2</v>
-      </c>
-      <c r="C44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
-      <c r="H44">
-        <f>LN(B44)</f>
-        <v>-2.7846613034740506</v>
-      </c>
-      <c r="I44">
-        <v>0.2</v>
-      </c>
-      <c r="N44" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45">
-        <v>0.38390999999999997</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <f>LN(B45)</f>
-        <v>-0.95734712886452289</v>
-      </c>
-      <c r="I45">
-        <v>0.2</v>
-      </c>
-      <c r="M45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46">
-        <v>0.38390999999999997</v>
-      </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
-      <c r="H46">
-        <f>LN(B46)</f>
-        <v>-0.95734712886452289</v>
-      </c>
-      <c r="I46">
-        <v>0.2</v>
-      </c>
-      <c r="M46" t="s">
-        <v>44</v>
-      </c>
-      <c r="N46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-      <c r="H47">
-        <f>B47</f>
-        <v>1</v>
-      </c>
-      <c r="M47" t="s">
+        <f>B43</f>
+        <v>1</v>
+      </c>
+      <c r="M43" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15">
-      <c r="A48" s="9"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" ht="15">
-      <c r="A49" s="9"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+    <row r="44" spans="1:14" ht="15">
+      <c r="A44" s="9"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" ht="15">
+      <c r="A45" s="9"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1981,7 +1957,7 @@
         <v>20</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>31</v>
@@ -2090,10 +2066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2110,216 +2086,198 @@
     <row r="1" spans="1:16">
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:16" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
+    <row r="2" spans="1:16">
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" ht="15">
-      <c r="A6" s="1" t="s">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:16" ht="15">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" ht="15">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" ht="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="P7" s="7"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="s">
-        <v>50</v>
+      <c r="A14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15">
+      <c r="A15" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
+      <c r="N15" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="15">
-      <c r="A16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16">
-        <v>0.5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15">
-      <c r="A17" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17">
-        <v>0.5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15">
-      <c r="D18" s="3"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2334,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2354,223 +2312,202 @@
     <row r="1" spans="1:14">
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>1</v>
+    <row r="3" spans="1:14" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="15">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
+      <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16">
-        <v>0.5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17">
-        <v>0.5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="D18" s="5"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add failing test for activating after the fact
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/sample_activities_with_variables.xlsx
+++ b/tests/fixtures/excel/sample_activities_with_variables.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10513"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/bw2/io/tests/fixtures/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{468BD2B4-FE3C-274C-8697-3F2BC3EE48C3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="795"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB inventory" sheetId="13" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>Database</t>
   </si>
@@ -157,15 +163,28 @@
   </si>
   <si>
     <t>alpha group!</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>mpcb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -239,110 +258,111 @@
   </borders>
   <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -740,27 +760,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="34.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -781,7 +801,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -800,7 +820,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -813,7 +833,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="15">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,7 +843,7 @@
       <c r="D5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -831,13 +851,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -872,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -892,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -912,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -932,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15">
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -940,148 +960,131 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
-      <c r="A17" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
-      <c r="A23" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B24" s="4">
         <v>0.6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" ht="15">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" t="s">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>33</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="N27" s="4"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" t="s">
-        <v>32</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>29</v>
@@ -1090,125 +1093,150 @@
         <v>24</v>
       </c>
       <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" t="s">
         <v>21</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" t="s">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" t="s">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
-      <c r="A33" t="s">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>5</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
-      <c r="A34" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
-      <c r="A35" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>7</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
-      <c r="A36" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" t="s">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>33</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>24</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>21</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>0</v>
       </c>
     </row>

</xml_diff>